<commit_message>
Change the data as sucess and in config file body has change
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -36,7 +36,7 @@
   </si>
   <si>
     <t>Hello {0},
-Hope your doing good, Please see attached Salary of Month {1}
+Hope you are doing well, Please see attached Salary of Month {1}
 Thank You!
 Nithya</t>
   </si>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>